<commit_message>
Added more result analysis files and sample images of the factory
</commit_message>
<xml_diff>
--- a/paper/documents/log25.xlsx
+++ b/paper/documents/log25.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="59">
   <si>
     <t>chemotactic Strength With Attract</t>
   </si>
@@ -145,6 +145,57 @@
   </si>
   <si>
     <t xml:space="preserve">  	 	0.0012574117899520453</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	3.408269787159056E-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	0.03720488968869235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	0.06418324651902178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	9.031411634719176E-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	5.133387916038291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	0.01568800014006551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	5.998373616196977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	0.049116719260224644</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	7.794854024412359E-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	5.521704510055601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	4.240628556678441E-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	3.8286276698093897</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	6.559039958995246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	0.0012217007069712767</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	6.279353044636841</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  	 	5.41672878927443E-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 472.35509400224385]</t>
   </si>
 </sst>
 </file>
@@ -800,10 +851,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>logCsv!$H$2:$H$63</c:f>
+              <c:f>logCsv!$H$2:$H$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="62"/>
+                <c:ptCount val="101"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -983,6 +1034,126 @@
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>280.34105413590601</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>269.81432051087398</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>280.34105413590601</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>261.40835232595998</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>261.40835232595998</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>280.34105413590601</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>403.69339294538099</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>261.40835232595998</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>280.34105413590601</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>327.52278838880898</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>270.82094471900899</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>261.40835232595998</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>403.69339294538099</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>377.04021491950499</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>375.95915135384303</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>362.80003751651702</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>403.69339294538099</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>403.69339294538099</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>400.81728556656401</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>403.69339294538099</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>435.47732332411903</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>403.23753476843598</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>472.35509400224299</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>403.69339294538099</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>403.69339294538099</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>472.35509400224299</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>435.47732332411903</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>419.808815527452</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>458.66983168607999</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>462.63863490090102</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>308.13683552983298</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>472.35509400224299</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>458.66983168607999</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>446.21100057756598</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>203.34111714248499</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>472.35509400224299</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>458.66983168607999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1227,7 +1398,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>logCsv!$A$64</c:f>
+              <c:f>logCsv!$A$103</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1256,10 +1427,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>logCsv!$B$64:$T$64</c:f>
+              <c:f>logCsv!$B$103:$AF$103</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1316,6 +1487,42 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>280.34105413590601</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>280.34105413590601</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>280.34105413590601</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>403.69339294538099</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>403.69339294538099</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>403.69339294538099</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>403.69339294538099</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>403.69339294538099</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>472.35509400224299</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>472.35509400224299</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>472.35509400224299</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>472.35509400224299</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>472.35509400224299</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2581,8 +2788,8 @@
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>390524</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
@@ -2611,8 +2818,8 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>400049</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -2933,10 +3140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T64"/>
+  <dimension ref="A1:AG103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:XFD47"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4186,7 +4393,7 @@
         <v>165.97910506150501</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>5.7301702160826604</v>
       </c>
@@ -4212,7 +4419,7 @@
         <v>245.54998455707101</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>5.7301702160826604</v>
       </c>
@@ -4238,7 +4445,7 @@
         <v>280.34105413590601</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>5.7301702160826604</v>
       </c>
@@ -4264,7 +4471,7 @@
         <v>280.34105413590601</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>5.7301702160826604</v>
       </c>
@@ -4290,7 +4497,7 @@
         <v>280.34105413590601</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>5.7301702160826604</v>
       </c>
@@ -4316,7 +4523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>5.7301702160826604</v>
       </c>
@@ -4342,7 +4549,7 @@
         <v>261.40835232595998</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>5.7301702160826604</v>
       </c>
@@ -4368,7 +4575,7 @@
         <v>280.34105413590601</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>5.7301702160826604</v>
       </c>
@@ -4394,7 +4601,7 @@
         <v>261.40835232595998</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>5.7301702160826604</v>
       </c>
@@ -4420,7 +4627,7 @@
         <v>261.40835232595998</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>5.7301702160826604</v>
       </c>
@@ -4446,7 +4653,7 @@
         <v>280.34105413590601</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>5.7301702160826604</v>
       </c>
@@ -4472,7 +4679,7 @@
         <v>280.34105413590601</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>5.7301702160826604</v>
       </c>
@@ -4498,7 +4705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>5.7301702160826604</v>
       </c>
@@ -4524,7 +4731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>5.7301702160826604</v>
       </c>
@@ -4550,7 +4757,7 @@
         <v>280.34105413590601</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>5.7301702160826604</v>
       </c>
@@ -4572,67 +4779,1123 @@
       <c r="G63" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="H63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>5.7301702160826604</v>
+      </c>
+      <c r="B64">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C64" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64" t="s">
+        <v>28</v>
+      </c>
+      <c r="F64" t="s">
+        <v>42</v>
+      </c>
+      <c r="G64" t="s">
+        <v>34</v>
+      </c>
+      <c r="H64">
+        <v>269.81432051087398</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>5.7301702160826604</v>
+      </c>
+      <c r="B65">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" t="s">
+        <v>19</v>
+      </c>
+      <c r="E65" t="s">
+        <v>28</v>
+      </c>
+      <c r="F65" t="s">
+        <v>11</v>
+      </c>
+      <c r="G65" t="s">
+        <v>34</v>
+      </c>
+      <c r="H65">
+        <v>280.34105413590601</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>5.7301702160826604</v>
+      </c>
+      <c r="B66">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C66" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" t="s">
+        <v>28</v>
+      </c>
+      <c r="F66" t="s">
+        <v>11</v>
+      </c>
+      <c r="G66" t="s">
+        <v>34</v>
+      </c>
+      <c r="H66">
+        <v>261.40835232595998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>5.7301702160826604</v>
+      </c>
+      <c r="B67">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C67" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" t="s">
+        <v>43</v>
+      </c>
+      <c r="F67" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" t="s">
+        <v>34</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>5.7301702160826604</v>
+      </c>
+      <c r="B68">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C68" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" t="s">
+        <v>28</v>
+      </c>
+      <c r="F68" t="s">
+        <v>11</v>
+      </c>
+      <c r="G68" t="s">
+        <v>34</v>
+      </c>
+      <c r="H68">
+        <v>261.40835232595998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>5.7301702160826604</v>
+      </c>
+      <c r="B69">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C69" t="s">
+        <v>18</v>
+      </c>
+      <c r="D69" t="s">
+        <v>19</v>
+      </c>
+      <c r="E69" t="s">
+        <v>28</v>
+      </c>
+      <c r="F69" t="s">
+        <v>11</v>
+      </c>
+      <c r="G69" t="s">
+        <v>34</v>
+      </c>
+      <c r="H69">
+        <v>280.34105413590601</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B70">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C70" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" t="s">
+        <v>28</v>
+      </c>
+      <c r="F70" t="s">
+        <v>11</v>
+      </c>
+      <c r="G70" t="s">
+        <v>34</v>
+      </c>
+      <c r="H70">
+        <v>403.69339294538099</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>5.7301702160826604</v>
+      </c>
+      <c r="B71">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C71" t="s">
+        <v>18</v>
+      </c>
+      <c r="D71" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" t="s">
+        <v>44</v>
+      </c>
+      <c r="F71" t="s">
+        <v>11</v>
+      </c>
+      <c r="G71" t="s">
+        <v>34</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>5.7301702160826604</v>
+      </c>
+      <c r="B72">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C72" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" t="s">
+        <v>28</v>
+      </c>
+      <c r="F72" t="s">
+        <v>11</v>
+      </c>
+      <c r="G72" t="s">
+        <v>34</v>
+      </c>
+      <c r="H72">
+        <v>261.40835232595998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>5.7301702160826604</v>
+      </c>
+      <c r="B73">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C73" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" t="s">
+        <v>19</v>
+      </c>
+      <c r="E73" t="s">
+        <v>28</v>
+      </c>
+      <c r="F73" t="s">
+        <v>11</v>
+      </c>
+      <c r="G73" t="s">
+        <v>34</v>
+      </c>
+      <c r="H73">
+        <v>280.34105413590601</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B74">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C74" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" t="s">
+        <v>28</v>
+      </c>
+      <c r="F74" t="s">
+        <v>45</v>
+      </c>
+      <c r="G74" t="s">
+        <v>34</v>
+      </c>
+      <c r="H74">
+        <v>327.52278838880898</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>5.7301702160826604</v>
+      </c>
+      <c r="B75">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C75" t="s">
+        <v>18</v>
+      </c>
+      <c r="D75" t="s">
+        <v>46</v>
+      </c>
+      <c r="E75" t="s">
+        <v>28</v>
+      </c>
+      <c r="F75" t="s">
+        <v>11</v>
+      </c>
+      <c r="G75" t="s">
+        <v>34</v>
+      </c>
+      <c r="H75">
+        <v>270.82094471900899</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>5.7301702160826604</v>
+      </c>
+      <c r="B76">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C76" t="s">
+        <v>18</v>
+      </c>
+      <c r="D76" t="s">
+        <v>19</v>
+      </c>
+      <c r="E76" t="s">
+        <v>28</v>
+      </c>
+      <c r="F76" t="s">
+        <v>11</v>
+      </c>
+      <c r="G76" t="s">
+        <v>34</v>
+      </c>
+      <c r="H76">
+        <v>261.40835232595998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B77">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C77" t="s">
+        <v>18</v>
+      </c>
+      <c r="D77" t="s">
+        <v>19</v>
+      </c>
+      <c r="E77" t="s">
+        <v>28</v>
+      </c>
+      <c r="F77" t="s">
+        <v>11</v>
+      </c>
+      <c r="G77" t="s">
+        <v>34</v>
+      </c>
+      <c r="H77">
+        <v>403.69339294538099</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>3.0102822016417399</v>
+      </c>
+      <c r="B78">
+        <v>3.86775347361379</v>
+      </c>
+      <c r="C78" t="s">
+        <v>18</v>
+      </c>
+      <c r="D78" t="s">
+        <v>19</v>
+      </c>
+      <c r="E78" t="s">
+        <v>47</v>
+      </c>
+      <c r="F78" t="s">
+        <v>11</v>
+      </c>
+      <c r="G78" t="s">
+        <v>34</v>
+      </c>
+      <c r="H78">
+        <v>377.04021491950499</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>3.0102822016417399</v>
+      </c>
+      <c r="B79">
+        <v>3.86775347361379</v>
+      </c>
+      <c r="C79" t="s">
+        <v>18</v>
+      </c>
+      <c r="D79" t="s">
+        <v>19</v>
+      </c>
+      <c r="E79" t="s">
+        <v>47</v>
+      </c>
+      <c r="F79" t="s">
+        <v>11</v>
+      </c>
+      <c r="G79" t="s">
+        <v>34</v>
+      </c>
+      <c r="H79">
+        <v>375.95915135384303</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>3.0102822016417399</v>
+      </c>
+      <c r="B80">
+        <v>3.86775347361379</v>
+      </c>
+      <c r="C80" t="s">
+        <v>18</v>
+      </c>
+      <c r="D80" t="s">
+        <v>19</v>
+      </c>
+      <c r="E80" t="s">
+        <v>47</v>
+      </c>
+      <c r="F80" t="s">
+        <v>11</v>
+      </c>
+      <c r="G80" t="s">
+        <v>34</v>
+      </c>
+      <c r="H80">
+        <v>362.80003751651702</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B81">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C81" t="s">
+        <v>18</v>
+      </c>
+      <c r="D81" t="s">
+        <v>19</v>
+      </c>
+      <c r="E81" t="s">
+        <v>28</v>
+      </c>
+      <c r="F81" t="s">
+        <v>11</v>
+      </c>
+      <c r="G81" t="s">
+        <v>34</v>
+      </c>
+      <c r="H81">
+        <v>403.69339294538099</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B82">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C82" t="s">
+        <v>18</v>
+      </c>
+      <c r="D82" t="s">
+        <v>19</v>
+      </c>
+      <c r="E82" t="s">
+        <v>28</v>
+      </c>
+      <c r="F82" t="s">
+        <v>11</v>
+      </c>
+      <c r="G82" t="s">
+        <v>34</v>
+      </c>
+      <c r="H82">
+        <v>403.69339294538099</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B83">
+        <v>2.2793884869889101</v>
+      </c>
+      <c r="C83" t="s">
+        <v>18</v>
+      </c>
+      <c r="D83" t="s">
+        <v>48</v>
+      </c>
+      <c r="E83" t="s">
+        <v>28</v>
+      </c>
+      <c r="F83" t="s">
+        <v>11</v>
+      </c>
+      <c r="G83" t="s">
+        <v>34</v>
+      </c>
+      <c r="H83">
+        <v>400.81728556656401</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B84">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C84" t="s">
+        <v>18</v>
+      </c>
+      <c r="D84" t="s">
+        <v>19</v>
+      </c>
+      <c r="E84" t="s">
+        <v>28</v>
+      </c>
+      <c r="F84" t="s">
+        <v>11</v>
+      </c>
+      <c r="G84" t="s">
+        <v>34</v>
+      </c>
+      <c r="H84">
+        <v>403.69339294538099</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B85">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C85" t="s">
+        <v>18</v>
+      </c>
+      <c r="D85" t="s">
+        <v>19</v>
+      </c>
+      <c r="E85" t="s">
+        <v>28</v>
+      </c>
+      <c r="F85" t="s">
+        <v>11</v>
+      </c>
+      <c r="G85" t="s">
+        <v>34</v>
+      </c>
+      <c r="H85">
+        <v>435.47732332411903</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B86">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C86" t="s">
+        <v>18</v>
+      </c>
+      <c r="D86" t="s">
+        <v>19</v>
+      </c>
+      <c r="E86" t="s">
+        <v>49</v>
+      </c>
+      <c r="F86" t="s">
+        <v>50</v>
+      </c>
+      <c r="G86" t="s">
+        <v>34</v>
+      </c>
+      <c r="H86">
+        <v>403.23753476843598</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B87">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C87" t="s">
+        <v>18</v>
+      </c>
+      <c r="D87" t="s">
+        <v>51</v>
+      </c>
+      <c r="E87" t="s">
+        <v>28</v>
+      </c>
+      <c r="F87" t="s">
+        <v>52</v>
+      </c>
+      <c r="G87" t="s">
+        <v>34</v>
+      </c>
+      <c r="H87">
+        <v>472.35509400224299</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B88">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C88" t="s">
+        <v>18</v>
+      </c>
+      <c r="D88" t="s">
+        <v>19</v>
+      </c>
+      <c r="E88" t="s">
+        <v>28</v>
+      </c>
+      <c r="F88" t="s">
+        <v>11</v>
+      </c>
+      <c r="G88" t="s">
+        <v>34</v>
+      </c>
+      <c r="H88">
+        <v>403.69339294538099</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B89">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C89" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89" t="s">
+        <v>19</v>
+      </c>
+      <c r="E89" t="s">
+        <v>28</v>
+      </c>
+      <c r="F89" t="s">
+        <v>11</v>
+      </c>
+      <c r="G89" t="s">
+        <v>34</v>
+      </c>
+      <c r="H89">
+        <v>403.69339294538099</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B90">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C90" t="s">
+        <v>18</v>
+      </c>
+      <c r="D90" t="s">
+        <v>51</v>
+      </c>
+      <c r="E90" t="s">
+        <v>28</v>
+      </c>
+      <c r="F90" t="s">
+        <v>52</v>
+      </c>
+      <c r="G90" t="s">
+        <v>34</v>
+      </c>
+      <c r="H90">
+        <v>472.35509400224299</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B91">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C91" t="s">
+        <v>18</v>
+      </c>
+      <c r="D91" t="s">
+        <v>19</v>
+      </c>
+      <c r="E91" t="s">
+        <v>28</v>
+      </c>
+      <c r="F91" t="s">
+        <v>11</v>
+      </c>
+      <c r="G91" t="s">
+        <v>34</v>
+      </c>
+      <c r="H91">
+        <v>435.47732332411903</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B92">
+        <v>5.5724916173989003</v>
+      </c>
+      <c r="C92" t="s">
+        <v>18</v>
+      </c>
+      <c r="D92" t="s">
+        <v>19</v>
+      </c>
+      <c r="E92" t="s">
+        <v>28</v>
+      </c>
+      <c r="F92" t="s">
+        <v>11</v>
+      </c>
+      <c r="G92" t="s">
+        <v>34</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B93">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C93" t="s">
+        <v>18</v>
+      </c>
+      <c r="D93" t="s">
+        <v>53</v>
+      </c>
+      <c r="E93" t="s">
+        <v>28</v>
+      </c>
+      <c r="F93" t="s">
+        <v>11</v>
+      </c>
+      <c r="G93" t="s">
+        <v>34</v>
+      </c>
+      <c r="H93">
+        <v>419.808815527452</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B94">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C94" t="s">
+        <v>18</v>
+      </c>
+      <c r="D94" t="s">
+        <v>51</v>
+      </c>
+      <c r="E94" t="s">
+        <v>28</v>
+      </c>
+      <c r="F94" t="s">
+        <v>52</v>
+      </c>
+      <c r="G94" t="s">
+        <v>34</v>
+      </c>
+      <c r="H94">
+        <v>458.66983168607999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B95">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C95" t="s">
+        <v>18</v>
+      </c>
+      <c r="D95" t="s">
+        <v>51</v>
+      </c>
+      <c r="E95" t="s">
+        <v>28</v>
+      </c>
+      <c r="F95" t="s">
+        <v>52</v>
+      </c>
+      <c r="G95" t="s">
+        <v>34</v>
+      </c>
+      <c r="H95">
+        <v>462.63863490090102</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B96">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C96" t="s">
+        <v>54</v>
+      </c>
+      <c r="D96" t="s">
+        <v>51</v>
+      </c>
+      <c r="E96" t="s">
+        <v>28</v>
+      </c>
+      <c r="F96" t="s">
+        <v>52</v>
+      </c>
+      <c r="G96" t="s">
+        <v>55</v>
+      </c>
+      <c r="H96">
+        <v>308.13683552983298</v>
+      </c>
+    </row>
+    <row r="97" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B97">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C97" t="s">
+        <v>18</v>
+      </c>
+      <c r="D97" t="s">
+        <v>51</v>
+      </c>
+      <c r="E97" t="s">
+        <v>28</v>
+      </c>
+      <c r="F97" t="s">
+        <v>52</v>
+      </c>
+      <c r="G97" t="s">
+        <v>34</v>
+      </c>
+      <c r="H97">
+        <v>472.35509400224299</v>
+      </c>
+    </row>
+    <row r="98" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B98">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C98" t="s">
+        <v>18</v>
+      </c>
+      <c r="D98" t="s">
+        <v>51</v>
+      </c>
+      <c r="E98" t="s">
+        <v>28</v>
+      </c>
+      <c r="F98" t="s">
+        <v>52</v>
+      </c>
+      <c r="G98" t="s">
+        <v>34</v>
+      </c>
+      <c r="H98">
+        <v>458.66983168607999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B99">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C99" t="s">
+        <v>56</v>
+      </c>
+      <c r="D99" t="s">
+        <v>51</v>
+      </c>
+      <c r="E99" t="s">
+        <v>28</v>
+      </c>
+      <c r="F99" t="s">
+        <v>52</v>
+      </c>
+      <c r="G99" t="s">
+        <v>34</v>
+      </c>
+      <c r="H99">
+        <v>446.21100057756598</v>
+      </c>
+    </row>
+    <row r="100" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B100">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C100" t="s">
+        <v>18</v>
+      </c>
+      <c r="D100" t="s">
+        <v>51</v>
+      </c>
+      <c r="E100" t="s">
+        <v>28</v>
+      </c>
+      <c r="F100" t="s">
+        <v>57</v>
+      </c>
+      <c r="G100" t="s">
+        <v>34</v>
+      </c>
+      <c r="H100">
+        <v>203.34111714248499</v>
+      </c>
+    </row>
+    <row r="101" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B101">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C101" t="s">
+        <v>18</v>
+      </c>
+      <c r="D101" t="s">
+        <v>51</v>
+      </c>
+      <c r="E101" t="s">
+        <v>28</v>
+      </c>
+      <c r="F101" t="s">
+        <v>52</v>
+      </c>
+      <c r="G101" t="s">
+        <v>34</v>
+      </c>
+      <c r="H101">
+        <v>472.35509400224299</v>
+      </c>
+    </row>
+    <row r="102" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>2.7270934416336701</v>
+      </c>
+      <c r="B102">
+        <v>1.56900652003531</v>
+      </c>
+      <c r="C102" t="s">
+        <v>18</v>
+      </c>
+      <c r="D102" t="s">
+        <v>51</v>
+      </c>
+      <c r="E102" t="s">
+        <v>28</v>
+      </c>
+      <c r="F102" t="s">
+        <v>52</v>
+      </c>
+      <c r="G102" t="s">
+        <v>34</v>
+      </c>
+      <c r="H102">
+        <v>458.66983168607999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>35</v>
       </c>
-      <c r="B64">
+      <c r="B103">
         <v>0</v>
       </c>
-      <c r="C64">
+      <c r="C103">
         <v>0</v>
       </c>
-      <c r="D64">
+      <c r="D103">
         <v>0</v>
       </c>
-      <c r="E64">
+      <c r="E103">
         <v>0</v>
       </c>
-      <c r="F64">
+      <c r="F103">
         <v>0</v>
       </c>
-      <c r="G64">
+      <c r="G103">
         <v>0</v>
       </c>
-      <c r="H64">
+      <c r="H103">
         <v>0</v>
       </c>
-      <c r="I64">
+      <c r="I103">
         <v>0</v>
       </c>
-      <c r="J64">
+      <c r="J103">
         <v>173.069712000457</v>
       </c>
-      <c r="K64">
+      <c r="K103">
         <v>173.069712000457</v>
       </c>
-      <c r="L64">
+      <c r="L103">
         <v>280.34105413590601</v>
       </c>
-      <c r="M64">
+      <c r="M103">
         <v>280.34105413590601</v>
       </c>
-      <c r="N64">
+      <c r="N103">
         <v>280.34105413590601</v>
       </c>
-      <c r="O64">
+      <c r="O103">
         <v>280.34105413590601</v>
       </c>
-      <c r="P64">
+      <c r="P103">
         <v>280.34105413590601</v>
       </c>
-      <c r="Q64">
+      <c r="Q103">
         <v>280.34105413590601</v>
       </c>
-      <c r="R64">
+      <c r="R103">
         <v>280.34105413590601</v>
       </c>
-      <c r="S64">
+      <c r="S103">
         <v>280.34105413590601</v>
       </c>
-      <c r="T64">
+      <c r="T103">
         <v>280.34105413590601</v>
+      </c>
+      <c r="U103">
+        <v>280.34105413590601</v>
+      </c>
+      <c r="V103">
+        <v>280.34105413590601</v>
+      </c>
+      <c r="W103">
+        <v>403.69339294538099</v>
+      </c>
+      <c r="X103">
+        <v>403.69339294538099</v>
+      </c>
+      <c r="Y103">
+        <v>403.69339294538099</v>
+      </c>
+      <c r="Z103">
+        <v>403.69339294538099</v>
+      </c>
+      <c r="AA103">
+        <v>403.69339294538099</v>
+      </c>
+      <c r="AB103">
+        <v>472.35509400224299</v>
+      </c>
+      <c r="AC103">
+        <v>472.35509400224299</v>
+      </c>
+      <c r="AD103">
+        <v>472.35509400224299</v>
+      </c>
+      <c r="AE103">
+        <v>472.35509400224299</v>
+      </c>
+      <c r="AF103">
+        <v>472.35509400224299</v>
+      </c>
+      <c r="AG103" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>